<commit_message>
Work on Nominations page
trying to get the drop down forms in nomination working. it is currently
now working but I have some usefull stuff in the scrappy.txt file
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -36,7 +36,7 @@
     <t>In the email field in the beginning there should be code to confirm that the email is entered correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">If there is nothing picked in the slot, there will be a zero entered into the nominations. </t>
+    <t>If there is nothing picked in the slot, there will be a zero entered into the nominations when the button is pressed</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>